<commit_message>
Adicionadas restantes tabelas de descontos de IRS
</commit_message>
<xml_diff>
--- a/Salários/Cópia de Tabelas_RF_Continente_2024.xlsx
+++ b/Salários/Cópia de Tabelas_RF_Continente_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcsil\Documents\Developing\Salários\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcsil\Documents\Developing\Calculadora de Salários\Salários\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A60BB793-77B7-4BBF-ADAF-2EB4CD18EE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D00A6EC-06F6-4F64-8877-05E5E36E6BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -685,10 +685,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1023,7 +1023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA285"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I129" sqref="I129"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1058,22 +1060,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
@@ -1090,22 +1092,22 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -1124,22 +1126,22 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1614,22 +1616,22 @@
       <c r="L24" s="26"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="114" t="s">
+      <c r="B25" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="114"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
-      <c r="G25" s="114"/>
-      <c r="H25" s="114"/>
-      <c r="I25" s="114"/>
-      <c r="J25" s="114"/>
-      <c r="K25" s="114"/>
-      <c r="L25" s="114"/>
-      <c r="M25" s="114"/>
-      <c r="N25" s="114"/>
-      <c r="O25" s="114"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="115"/>
+      <c r="K25" s="115"/>
+      <c r="L25" s="115"/>
+      <c r="M25" s="115"/>
+      <c r="N25" s="115"/>
+      <c r="O25" s="115"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -1648,22 +1650,22 @@
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="114" t="s">
+      <c r="B27" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="114"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="114"/>
-      <c r="O27" s="114"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
+      <c r="N27" s="115"/>
+      <c r="O27" s="115"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,41 +2140,41 @@
       <c r="L46" s="26"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="115" t="s">
+      <c r="B47" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="115"/>
-      <c r="D47" s="115"/>
-      <c r="E47" s="115"/>
-      <c r="F47" s="115"/>
-      <c r="G47" s="115"/>
-      <c r="H47" s="115"/>
-      <c r="I47" s="115"/>
-      <c r="J47" s="115"/>
-      <c r="K47" s="115"/>
-      <c r="L47" s="115"/>
-      <c r="M47" s="115"/>
-      <c r="N47" s="115"/>
-      <c r="O47" s="115"/>
+      <c r="C47" s="114"/>
+      <c r="D47" s="114"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="114"/>
+      <c r="G47" s="114"/>
+      <c r="H47" s="114"/>
+      <c r="I47" s="114"/>
+      <c r="J47" s="114"/>
+      <c r="K47" s="114"/>
+      <c r="L47" s="114"/>
+      <c r="M47" s="114"/>
+      <c r="N47" s="114"/>
+      <c r="O47" s="114"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="114" t="s">
+      <c r="B49" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="114"/>
-      <c r="D49" s="114"/>
-      <c r="E49" s="114"/>
-      <c r="F49" s="114"/>
-      <c r="G49" s="114"/>
-      <c r="H49" s="114"/>
-      <c r="I49" s="114"/>
-      <c r="J49" s="114"/>
-      <c r="K49" s="114"/>
-      <c r="L49" s="114"/>
-      <c r="M49" s="114"/>
-      <c r="N49" s="114"/>
-      <c r="O49" s="114"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="115"/>
+      <c r="E49" s="115"/>
+      <c r="F49" s="115"/>
+      <c r="G49" s="115"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="115"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="115"/>
+      <c r="L49" s="115"/>
+      <c r="M49" s="115"/>
+      <c r="N49" s="115"/>
+      <c r="O49" s="115"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:20" s="48" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2613,22 +2615,22 @@
       <c r="L67" s="26"/>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="115" t="s">
+      <c r="B68" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="115"/>
-      <c r="D68" s="115"/>
-      <c r="E68" s="115"/>
-      <c r="F68" s="115"/>
-      <c r="G68" s="115"/>
-      <c r="H68" s="115"/>
-      <c r="I68" s="115"/>
-      <c r="J68" s="115"/>
-      <c r="K68" s="115"/>
-      <c r="L68" s="115"/>
-      <c r="M68" s="115"/>
-      <c r="N68" s="115"/>
-      <c r="O68" s="115"/>
+      <c r="C68" s="114"/>
+      <c r="D68" s="114"/>
+      <c r="E68" s="114"/>
+      <c r="F68" s="114"/>
+      <c r="G68" s="114"/>
+      <c r="H68" s="114"/>
+      <c r="I68" s="114"/>
+      <c r="J68" s="114"/>
+      <c r="K68" s="114"/>
+      <c r="L68" s="114"/>
+      <c r="M68" s="114"/>
+      <c r="N68" s="114"/>
+      <c r="O68" s="114"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B69" s="62"/>
@@ -2644,22 +2646,22 @@
       <c r="L69" s="62"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="114" t="s">
+      <c r="B70" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="114"/>
-      <c r="D70" s="114"/>
-      <c r="E70" s="114"/>
-      <c r="F70" s="114"/>
-      <c r="G70" s="114"/>
-      <c r="H70" s="114"/>
-      <c r="I70" s="114"/>
-      <c r="J70" s="114"/>
-      <c r="K70" s="114"/>
-      <c r="L70" s="114"/>
-      <c r="M70" s="114"/>
-      <c r="N70" s="114"/>
-      <c r="O70" s="114"/>
+      <c r="C70" s="115"/>
+      <c r="D70" s="115"/>
+      <c r="E70" s="115"/>
+      <c r="F70" s="115"/>
+      <c r="G70" s="115"/>
+      <c r="H70" s="115"/>
+      <c r="I70" s="115"/>
+      <c r="J70" s="115"/>
+      <c r="K70" s="115"/>
+      <c r="L70" s="115"/>
+      <c r="M70" s="115"/>
+      <c r="N70" s="115"/>
+      <c r="O70" s="115"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:15" ht="45" x14ac:dyDescent="0.25">
@@ -2956,41 +2958,41 @@
       <c r="L85" s="113"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="115" t="s">
+      <c r="B86" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="C86" s="115"/>
-      <c r="D86" s="115"/>
-      <c r="E86" s="115"/>
-      <c r="F86" s="115"/>
-      <c r="G86" s="115"/>
-      <c r="H86" s="115"/>
-      <c r="I86" s="115"/>
-      <c r="J86" s="115"/>
-      <c r="K86" s="115"/>
-      <c r="L86" s="115"/>
-      <c r="M86" s="115"/>
-      <c r="N86" s="115"/>
-      <c r="O86" s="115"/>
+      <c r="C86" s="114"/>
+      <c r="D86" s="114"/>
+      <c r="E86" s="114"/>
+      <c r="F86" s="114"/>
+      <c r="G86" s="114"/>
+      <c r="H86" s="114"/>
+      <c r="I86" s="114"/>
+      <c r="J86" s="114"/>
+      <c r="K86" s="114"/>
+      <c r="L86" s="114"/>
+      <c r="M86" s="114"/>
+      <c r="N86" s="114"/>
+      <c r="O86" s="114"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="114" t="s">
+      <c r="B88" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="C88" s="114"/>
-      <c r="D88" s="114"/>
-      <c r="E88" s="114"/>
-      <c r="F88" s="114"/>
-      <c r="G88" s="114"/>
-      <c r="H88" s="114"/>
-      <c r="I88" s="114"/>
-      <c r="J88" s="114"/>
-      <c r="K88" s="114"/>
-      <c r="L88" s="114"/>
-      <c r="M88" s="114"/>
-      <c r="N88" s="114"/>
-      <c r="O88" s="114"/>
+      <c r="C88" s="115"/>
+      <c r="D88" s="115"/>
+      <c r="E88" s="115"/>
+      <c r="F88" s="115"/>
+      <c r="G88" s="115"/>
+      <c r="H88" s="115"/>
+      <c r="I88" s="115"/>
+      <c r="J88" s="115"/>
+      <c r="K88" s="115"/>
+      <c r="L88" s="115"/>
+      <c r="M88" s="115"/>
+      <c r="N88" s="115"/>
+      <c r="O88" s="115"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:15" ht="60" x14ac:dyDescent="0.25">
@@ -3303,41 +3305,41 @@
       <c r="L102" s="26"/>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B103" s="115" t="s">
+      <c r="B103" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C103" s="115"/>
-      <c r="D103" s="115"/>
-      <c r="E103" s="115"/>
-      <c r="F103" s="115"/>
-      <c r="G103" s="115"/>
-      <c r="H103" s="115"/>
-      <c r="I103" s="115"/>
-      <c r="J103" s="115"/>
-      <c r="K103" s="115"/>
-      <c r="L103" s="115"/>
-      <c r="M103" s="115"/>
-      <c r="N103" s="115"/>
-      <c r="O103" s="115"/>
+      <c r="C103" s="114"/>
+      <c r="D103" s="114"/>
+      <c r="E103" s="114"/>
+      <c r="F103" s="114"/>
+      <c r="G103" s="114"/>
+      <c r="H103" s="114"/>
+      <c r="I103" s="114"/>
+      <c r="J103" s="114"/>
+      <c r="K103" s="114"/>
+      <c r="L103" s="114"/>
+      <c r="M103" s="114"/>
+      <c r="N103" s="114"/>
+      <c r="O103" s="114"/>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25"/>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B105" s="114" t="s">
+      <c r="B105" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="C105" s="114"/>
-      <c r="D105" s="114"/>
-      <c r="E105" s="114"/>
-      <c r="F105" s="114"/>
-      <c r="G105" s="114"/>
-      <c r="H105" s="114"/>
-      <c r="I105" s="114"/>
-      <c r="J105" s="114"/>
-      <c r="K105" s="114"/>
-      <c r="L105" s="114"/>
-      <c r="M105" s="114"/>
-      <c r="N105" s="114"/>
-      <c r="O105" s="114"/>
+      <c r="C105" s="115"/>
+      <c r="D105" s="115"/>
+      <c r="E105" s="115"/>
+      <c r="F105" s="115"/>
+      <c r="G105" s="115"/>
+      <c r="H105" s="115"/>
+      <c r="I105" s="115"/>
+      <c r="J105" s="115"/>
+      <c r="K105" s="115"/>
+      <c r="L105" s="115"/>
+      <c r="M105" s="115"/>
+      <c r="N105" s="115"/>
+      <c r="O105" s="115"/>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25"/>
     <row r="107" spans="1:20" s="48" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -3684,41 +3686,41 @@
       <c r="L120" s="26"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B121" s="115" t="s">
+      <c r="B121" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="C121" s="115"/>
-      <c r="D121" s="115"/>
-      <c r="E121" s="115"/>
-      <c r="F121" s="115"/>
-      <c r="G121" s="115"/>
-      <c r="H121" s="115"/>
-      <c r="I121" s="115"/>
-      <c r="J121" s="115"/>
-      <c r="K121" s="115"/>
-      <c r="L121" s="115"/>
-      <c r="M121" s="115"/>
-      <c r="N121" s="115"/>
-      <c r="O121" s="115"/>
+      <c r="C121" s="114"/>
+      <c r="D121" s="114"/>
+      <c r="E121" s="114"/>
+      <c r="F121" s="114"/>
+      <c r="G121" s="114"/>
+      <c r="H121" s="114"/>
+      <c r="I121" s="114"/>
+      <c r="J121" s="114"/>
+      <c r="K121" s="114"/>
+      <c r="L121" s="114"/>
+      <c r="M121" s="114"/>
+      <c r="N121" s="114"/>
+      <c r="O121" s="114"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B123" s="114" t="s">
+      <c r="B123" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="C123" s="114"/>
-      <c r="D123" s="114"/>
-      <c r="E123" s="114"/>
-      <c r="F123" s="114"/>
-      <c r="G123" s="114"/>
-      <c r="H123" s="114"/>
-      <c r="I123" s="114"/>
-      <c r="J123" s="114"/>
-      <c r="K123" s="114"/>
-      <c r="L123" s="114"/>
-      <c r="M123" s="114"/>
-      <c r="N123" s="114"/>
-      <c r="O123" s="114"/>
+      <c r="C123" s="115"/>
+      <c r="D123" s="115"/>
+      <c r="E123" s="115"/>
+      <c r="F123" s="115"/>
+      <c r="G123" s="115"/>
+      <c r="H123" s="115"/>
+      <c r="I123" s="115"/>
+      <c r="J123" s="115"/>
+      <c r="K123" s="115"/>
+      <c r="L123" s="115"/>
+      <c r="M123" s="115"/>
+      <c r="N123" s="115"/>
+      <c r="O123" s="115"/>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="125" spans="2:15" ht="60" x14ac:dyDescent="0.25">
@@ -6571,23 +6573,21 @@
     <row r="285" spans="2:20" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B133:L133"/>
-    <mergeCell ref="B119:L119"/>
-    <mergeCell ref="B120:J120"/>
-    <mergeCell ref="B121:O121"/>
-    <mergeCell ref="B123:O123"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="G125:L125"/>
-    <mergeCell ref="B103:O103"/>
-    <mergeCell ref="B105:O105"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="G107:L107"/>
-    <mergeCell ref="B118:O118"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="G90:L90"/>
-    <mergeCell ref="B100:O100"/>
-    <mergeCell ref="B101:L101"/>
-    <mergeCell ref="B102:J102"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B25:O25"/>
+    <mergeCell ref="B27:O27"/>
+    <mergeCell ref="B44:O44"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B47:O47"/>
+    <mergeCell ref="B49:O49"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="G51:L51"/>
+    <mergeCell ref="B65:O65"/>
     <mergeCell ref="B88:O88"/>
     <mergeCell ref="B66:L66"/>
     <mergeCell ref="B67:J67"/>
@@ -6599,21 +6599,23 @@
     <mergeCell ref="B84:L84"/>
     <mergeCell ref="B85:L85"/>
     <mergeCell ref="B86:O86"/>
-    <mergeCell ref="B47:O47"/>
-    <mergeCell ref="B49:O49"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="G51:L51"/>
-    <mergeCell ref="B65:O65"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B25:O25"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="B44:O44"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B5:O5"/>
-    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="G90:L90"/>
+    <mergeCell ref="B100:O100"/>
+    <mergeCell ref="B101:L101"/>
+    <mergeCell ref="B102:J102"/>
+    <mergeCell ref="B103:O103"/>
+    <mergeCell ref="B105:O105"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="G107:L107"/>
+    <mergeCell ref="B118:O118"/>
+    <mergeCell ref="B133:L133"/>
+    <mergeCell ref="B119:L119"/>
+    <mergeCell ref="B120:J120"/>
+    <mergeCell ref="B121:O121"/>
+    <mergeCell ref="B123:O123"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="G125:L125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6654,60 +6656,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
     </row>
     <row r="2" spans="2:15" ht="15" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
+      <c r="M3" s="115"/>
+      <c r="N3" s="115"/>
+      <c r="O3" s="115"/>
     </row>
     <row r="4" spans="2:15" ht="15" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
     </row>
     <row r="6" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="N6" s="5"/>
@@ -7164,41 +7166,41 @@
       <c r="O24" s="5"/>
     </row>
     <row r="25" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="114" t="s">
+      <c r="B25" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="114"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
-      <c r="G25" s="114"/>
-      <c r="H25" s="114"/>
-      <c r="I25" s="114"/>
-      <c r="J25" s="114"/>
-      <c r="K25" s="114"/>
-      <c r="L25" s="114"/>
-      <c r="M25" s="114"/>
-      <c r="N25" s="114"/>
-      <c r="O25" s="114"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="115"/>
+      <c r="K25" s="115"/>
+      <c r="L25" s="115"/>
+      <c r="M25" s="115"/>
+      <c r="N25" s="115"/>
+      <c r="O25" s="115"/>
     </row>
     <row r="26" spans="2:15" ht="15" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="114" t="s">
+      <c r="B27" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="114"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="114"/>
-      <c r="O27" s="114"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
+      <c r="N27" s="115"/>
+      <c r="O27" s="115"/>
     </row>
     <row r="28" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="N28" s="5"/>
@@ -7655,41 +7657,41 @@
       <c r="O46" s="5"/>
     </row>
     <row r="47" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="114" t="s">
+      <c r="B47" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="114"/>
-      <c r="D47" s="114"/>
-      <c r="E47" s="114"/>
-      <c r="F47" s="114"/>
-      <c r="G47" s="114"/>
-      <c r="H47" s="114"/>
-      <c r="I47" s="114"/>
-      <c r="J47" s="114"/>
-      <c r="K47" s="114"/>
-      <c r="L47" s="114"/>
-      <c r="M47" s="114"/>
-      <c r="N47" s="114"/>
-      <c r="O47" s="114"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="115"/>
+      <c r="J47" s="115"/>
+      <c r="K47" s="115"/>
+      <c r="L47" s="115"/>
+      <c r="M47" s="115"/>
+      <c r="N47" s="115"/>
+      <c r="O47" s="115"/>
     </row>
     <row r="48" spans="2:15" ht="15" x14ac:dyDescent="0.25"/>
     <row r="49" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="114" t="s">
+      <c r="B49" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="114"/>
-      <c r="D49" s="114"/>
-      <c r="E49" s="114"/>
-      <c r="F49" s="114"/>
-      <c r="G49" s="114"/>
-      <c r="H49" s="114"/>
-      <c r="I49" s="114"/>
-      <c r="J49" s="114"/>
-      <c r="K49" s="114"/>
-      <c r="L49" s="114"/>
-      <c r="M49" s="114"/>
-      <c r="N49" s="114"/>
-      <c r="O49" s="114"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="115"/>
+      <c r="E49" s="115"/>
+      <c r="F49" s="115"/>
+      <c r="G49" s="115"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="115"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="115"/>
+      <c r="L49" s="115"/>
+      <c r="M49" s="115"/>
+      <c r="N49" s="115"/>
+      <c r="O49" s="115"/>
     </row>
     <row r="50" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="N50" s="5"/>
@@ -8029,41 +8031,41 @@
       <c r="M64" s="44"/>
     </row>
     <row r="65" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="114" t="s">
+      <c r="B65" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C65" s="114"/>
-      <c r="D65" s="114"/>
-      <c r="E65" s="114"/>
-      <c r="F65" s="114"/>
-      <c r="G65" s="114"/>
-      <c r="H65" s="114"/>
-      <c r="I65" s="114"/>
-      <c r="J65" s="114"/>
-      <c r="K65" s="114"/>
-      <c r="L65" s="114"/>
-      <c r="M65" s="114"/>
-      <c r="N65" s="114"/>
-      <c r="O65" s="114"/>
+      <c r="C65" s="115"/>
+      <c r="D65" s="115"/>
+      <c r="E65" s="115"/>
+      <c r="F65" s="115"/>
+      <c r="G65" s="115"/>
+      <c r="H65" s="115"/>
+      <c r="I65" s="115"/>
+      <c r="J65" s="115"/>
+      <c r="K65" s="115"/>
+      <c r="L65" s="115"/>
+      <c r="M65" s="115"/>
+      <c r="N65" s="115"/>
+      <c r="O65" s="115"/>
     </row>
     <row r="66" spans="2:15" ht="15" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="114" t="s">
+      <c r="B67" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="114"/>
-      <c r="D67" s="114"/>
-      <c r="E67" s="114"/>
-      <c r="F67" s="114"/>
-      <c r="G67" s="114"/>
-      <c r="H67" s="114"/>
-      <c r="I67" s="114"/>
-      <c r="J67" s="114"/>
-      <c r="K67" s="114"/>
-      <c r="L67" s="114"/>
-      <c r="M67" s="114"/>
-      <c r="N67" s="114"/>
-      <c r="O67" s="114"/>
+      <c r="C67" s="115"/>
+      <c r="D67" s="115"/>
+      <c r="E67" s="115"/>
+      <c r="F67" s="115"/>
+      <c r="G67" s="115"/>
+      <c r="H67" s="115"/>
+      <c r="I67" s="115"/>
+      <c r="J67" s="115"/>
+      <c r="K67" s="115"/>
+      <c r="L67" s="115"/>
+      <c r="M67" s="115"/>
+      <c r="N67" s="115"/>
+      <c r="O67" s="115"/>
     </row>
     <row r="68" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="N68" s="5"/>
@@ -8408,21 +8410,6 @@
     <row r="86" spans="2:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B81:L81"/>
-    <mergeCell ref="B82:L82"/>
-    <mergeCell ref="B65:O65"/>
-    <mergeCell ref="B67:O67"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="G69:L69"/>
-    <mergeCell ref="B64:L64"/>
-    <mergeCell ref="B44:L44"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:O47"/>
-    <mergeCell ref="B49:O49"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="G51:L51"/>
-    <mergeCell ref="B63:L63"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G29:L29"/>
     <mergeCell ref="B1:O1"/>
@@ -8435,6 +8422,21 @@
     <mergeCell ref="B24:L24"/>
     <mergeCell ref="B25:O25"/>
     <mergeCell ref="B27:O27"/>
+    <mergeCell ref="B64:L64"/>
+    <mergeCell ref="B44:L44"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:O47"/>
+    <mergeCell ref="B49:O49"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="G51:L51"/>
+    <mergeCell ref="B63:L63"/>
+    <mergeCell ref="B81:L81"/>
+    <mergeCell ref="B82:L82"/>
+    <mergeCell ref="B65:O65"/>
+    <mergeCell ref="B67:O67"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="G69:L69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8863,6 +8865,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_x00c1_rea xmlns="b8295a9a-ea95-40d3-b07e-7f4164936848" xsi:nil="true"/>
@@ -8879,15 +8890,6 @@
     <NOrdem xmlns="b8295a9a-ea95-40d3-b07e-7f4164936848" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8911,6 +8913,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{987EB98E-6C44-4649-9F6A-6A990988AE76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E76EE18-A9DE-468E-90B4-6FEBECDF11D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8920,12 +8930,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{987EB98E-6C44-4649-9F6A-6A990988AE76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>